<commit_message>
voltando a daily 25/09
</commit_message>
<xml_diff>
--- a/reuniões/dailys/Daily_25_09.xlsx
+++ b/reuniões/dailys/Daily_25_09.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="57" documentId="8_{10D53E0E-8B33-4524-B353-73D42DE15BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D2A983E-64D3-434F-B4E8-4612B039E61F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{10D53E0E-8B33-4524-B353-73D42DE15BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>AGENDA DE REUNIÕES ORCHIS SYSTEM</t>
   </si>
@@ -108,6 +108,12 @@
     <t>Replanejamento de Entregavéis</t>
   </si>
   <si>
+    <t>Atribuição de novas tarefas</t>
+  </si>
+  <si>
+    <t>Discussão de andamento do Projeto</t>
+  </si>
+  <si>
     <t>Criação da Tela Home</t>
   </si>
   <si>
@@ -127,24 +133,6 @@
   </si>
   <si>
     <t>Instalação MYSQL na VM</t>
-  </si>
-  <si>
-    <t>Concluído</t>
-  </si>
-  <si>
-    <t>Criação da Tela Sobre Nós</t>
-  </si>
-  <si>
-    <t>Planilha de Risco</t>
-  </si>
-  <si>
-    <t>Estilização Simulador</t>
-  </si>
-  <si>
-    <t>Inserção de Dados na VM</t>
-  </si>
-  <si>
-    <t>Planejamento Sprint 2B</t>
   </si>
 </sst>
 </file>
@@ -715,7 +703,7 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -740,6 +728,9 @@
     <xf numFmtId="166" fontId="18" fillId="32" borderId="0" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
+    <xf numFmtId="166" fontId="18" fillId="32" borderId="0" xfId="14" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
@@ -811,15 +802,6 @@
     </xf>
     <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="13" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="32" borderId="0" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="32" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="32" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -875,54 +857,6 @@
     <cellStyle name="Vírgula" xfId="1" builtinId="3" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="18">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <name val="Poppins"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <name val="Poppins"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF922A74"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1091,6 +1025,54 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor rgb="FFEFD5EC"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Poppins"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Poppins"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF922A74"/>
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1395,12 +1377,16 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="DadosDaReunião" displayName="DadosDaReunião" ref="B8:C18" totalsRowCount="1" headerRowDxfId="17" dataDxfId="16" totalsRowDxfId="15">
   <autoFilter ref="B8:C17" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="2">
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Assuntos Discutidos" dataDxfId="14" totalsRowDxfId="1" dataCellStyle="Normal"/>
-    <tableColumn id="6" xr3:uid="{19E48FEE-BF0F-4F91-A6DF-64EF1072BC46}" name="Presentes" dataDxfId="13" totalsRowDxfId="0" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Assuntos Discutidos" dataDxfId="14" totalsRowDxfId="9" dataCellStyle="Normal"/>
+    <tableColumn id="6" xr3:uid="{19E48FEE-BF0F-4F91-A6DF-64EF1072BC46}" name="Presentes" dataDxfId="13" totalsRowDxfId="8" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
   <extLst>
@@ -1412,17 +1398,17 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CE37D6C8-AC04-46A6-AAA6-24B204D1D210}" name="DadosDaReunião2" displayName="DadosDaReunião2" ref="B21:E33" totalsRowCount="1" headerRowDxfId="12" dataDxfId="11" totalsRowDxfId="10">
-  <autoFilter ref="B21:E32" xr:uid="{CE37D6C8-AC04-46A6-AAA6-24B204D1D210}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CE37D6C8-AC04-46A6-AAA6-24B204D1D210}" name="DadosDaReunião2" displayName="DadosDaReunião2" ref="B21:E31" totalsRowCount="1" headerRowDxfId="12" dataDxfId="11" totalsRowDxfId="10">
+  <autoFilter ref="B21:E30" xr:uid="{CE37D6C8-AC04-46A6-AAA6-24B204D1D210}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{BCB40325-DDE7-4562-A460-C0F89FD9179B}" name="Atividades" dataDxfId="9" totalsRowDxfId="5" dataCellStyle="Horário de Início/Término">
+    <tableColumn id="1" xr3:uid="{BCB40325-DDE7-4562-A460-C0F89FD9179B}" name="Atividades" dataDxfId="7" totalsRowDxfId="3" dataCellStyle="Horário de Início/Término">
       <calculatedColumnFormula>IF(ISBLANK(C21),"",C21)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{93D62D18-C90E-48BF-B30A-D911F7A6FCD8}" name="Entrega" dataDxfId="8" totalsRowDxfId="4" dataCellStyle="Horário de Início/Término">
+    <tableColumn id="2" xr3:uid="{93D62D18-C90E-48BF-B30A-D911F7A6FCD8}" name="Entrega" dataDxfId="6" totalsRowDxfId="2" dataCellStyle="Horário de Início/Término">
       <calculatedColumnFormula>IFERROR(IF(ISBLANK(D22),"",B22+D22), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{C88724A6-1AAA-442A-AC5D-FA9CC640F437}" name="Responsável" dataDxfId="7" totalsRowDxfId="3" dataCellStyle="Hora"/>
-    <tableColumn id="4" xr3:uid="{9E5AC715-A849-49E0-86B6-4B41F726ED66}" name="Situação" dataDxfId="6" totalsRowDxfId="2" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{C88724A6-1AAA-442A-AC5D-FA9CC640F437}" name="Responsável" dataDxfId="5" totalsRowDxfId="1" dataCellStyle="Hora"/>
+    <tableColumn id="4" xr3:uid="{9E5AC715-A849-49E0-86B6-4B41F726ED66}" name="Situação" dataDxfId="4" totalsRowDxfId="0" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
   <extLst>
@@ -1664,10 +1650,10 @@
     <tabColor theme="8"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:I33"/>
+  <dimension ref="B1:I31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B2" zoomScale="88" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="30" customHeight="1"/>
@@ -1688,54 +1674,54 @@
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="2:9" ht="60" customHeight="1">
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
     </row>
     <row r="3" spans="2:9" ht="30" customHeight="1">
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="31"/>
+      <c r="C3" s="32"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="2:9" ht="30" customHeight="1">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="18" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="2"/>
-      <c r="E4" s="20"/>
+      <c r="E4" s="21"/>
     </row>
     <row r="5" spans="2:9" ht="30" customHeight="1">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="19" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="E5" s="21"/>
+      <c r="E5" s="22"/>
     </row>
     <row r="6" spans="2:9" ht="30" customHeight="1">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="19">
-        <v>45561</v>
+      <c r="C6" s="20">
+        <v>45560</v>
       </c>
       <c r="D6" s="4"/>
-      <c r="E6" s="22"/>
+      <c r="E6" s="23"/>
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="2:9" ht="30" customHeight="1">
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="14" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="5"/>
@@ -1746,67 +1732,69 @@
       <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="21.6" customHeight="1">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="30" customHeight="1">
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="30" customHeight="1">
-      <c r="B11" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="8" t="s">
+      <c r="B11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="2:9" ht="30" customHeight="1">
-      <c r="B12" s="8"/>
-      <c r="C12" s="8" t="s">
+      <c r="B12" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="2:9" ht="30" customHeight="1">
-      <c r="B13" s="8"/>
-      <c r="C13" s="8" t="s">
+      <c r="B13" s="9"/>
+      <c r="C13" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="30" customHeight="1">
-      <c r="B14" s="8"/>
-      <c r="C14" s="8" t="s">
+      <c r="B14" s="9"/>
+      <c r="C14" s="9" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="30" customHeight="1">
-      <c r="B15" s="8"/>
-      <c r="C15" s="25"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="26"/>
     </row>
     <row r="16" spans="2:9" ht="30" customHeight="1">
-      <c r="B16" s="8"/>
-      <c r="C16" s="23"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="24"/>
     </row>
     <row r="17" spans="2:5" ht="30" customHeight="1">
-      <c r="B17" s="8"/>
-      <c r="C17" s="23"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="24"/>
     </row>
     <row r="18" spans="2:5" ht="30" customHeight="1">
-      <c r="B18" s="10"/>
-      <c r="C18" s="24"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="25"/>
     </row>
     <row r="19" spans="2:5" ht="30" customHeight="1">
       <c r="B19" s="1"/>
@@ -1815,7 +1803,7 @@
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="2:5" ht="30" customHeight="1">
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="14" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="1"/>
@@ -1838,158 +1826,111 @@
     </row>
     <row r="22" spans="2:5" ht="30" customHeight="1">
       <c r="B22" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="26">
+        <v>25</v>
+      </c>
+      <c r="C22" s="27">
         <v>45561</v>
       </c>
-      <c r="D22" s="28" t="s">
+      <c r="D22" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="8" t="s">
-        <v>30</v>
+      <c r="E22" s="9" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="30" customHeight="1">
       <c r="B23" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="27">
+        <v>27</v>
+      </c>
+      <c r="C23" s="28">
         <v>45561</v>
       </c>
-      <c r="D23" s="28" t="s">
+      <c r="D23" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="8" t="s">
-        <v>30</v>
+      <c r="E23" s="9" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="2:5" ht="30" customHeight="1">
       <c r="B24" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="28">
+        <v>45561</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="9" t="s">
         <v>26</v>
-      </c>
-      <c r="C24" s="27">
-        <v>45561</v>
-      </c>
-      <c r="D24" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="25" spans="2:5" ht="30" customHeight="1">
       <c r="B25" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="27">
-        <v>45568</v>
-      </c>
-      <c r="D25" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="28">
+        <v>45561</v>
+      </c>
+      <c r="D25" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E25" s="8" t="s">
-        <v>24</v>
+      <c r="E25" s="9" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="30" customHeight="1">
       <c r="B26" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="27">
-        <v>45568</v>
-      </c>
-      <c r="D26" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="28">
+        <v>45561</v>
+      </c>
+      <c r="D26" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="8" t="s">
-        <v>24</v>
+      <c r="E26" s="9" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="2:5" ht="30" customHeight="1">
       <c r="B27" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="27">
+        <v>31</v>
+      </c>
+      <c r="C27" s="28">
         <v>45561</v>
       </c>
-      <c r="D27" s="28" t="s">
+      <c r="D27" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="E27" s="8" t="s">
-        <v>30</v>
+      <c r="E27" s="9" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="2:5" ht="30" customHeight="1">
-      <c r="B28" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C28" s="27">
-        <v>45568</v>
-      </c>
-      <c r="D28" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>24</v>
-      </c>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="9"/>
     </row>
     <row r="29" spans="2:5" ht="30" customHeight="1">
-      <c r="B29" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29" s="27">
-        <v>45568</v>
-      </c>
-      <c r="D29" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>24</v>
-      </c>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="9"/>
     </row>
     <row r="30" spans="2:5" ht="30" customHeight="1">
-      <c r="B30" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" s="27">
-        <v>45568</v>
-      </c>
-      <c r="D30" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>24</v>
-      </c>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="9"/>
     </row>
     <row r="31" spans="2:5" ht="30" customHeight="1">
-      <c r="B31" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="C31" s="27">
-        <v>45568</v>
-      </c>
-      <c r="D31" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" ht="30" customHeight="1">
-      <c r="B32" s="32"/>
-      <c r="C32" s="32" t="str">
-        <f>IFERROR(IF(ISBLANK(D32),"",B32+D32), "")</f>
-        <v/>
-      </c>
-      <c r="D32" s="33"/>
-      <c r="E32" s="8"/>
-    </row>
-    <row r="33" spans="2:5" ht="30" customHeight="1">
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="12"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2182,20 +2123,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="9fdc8751-6fef-42ec-b05c-835dd8c535b4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="9fdc8751-6fef-42ec-b05c-835dd8c535b4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2217,6 +2158,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F57C8022-9D6B-4416-AED0-B410FD575972}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{932E6384-755C-48D1-BEC1-844EA204F516}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2226,14 +2175,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F57C8022-9D6B-4416-AED0-B410FD575972}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>